<commit_message>
Updated support MX Excel
</commit_message>
<xml_diff>
--- a/problems/11/preview_addr.xlsx
+++ b/problems/11/preview_addr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huski/Documents/R Projects/Euler/problems/11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E40CA8B-8D47-1C4E-8364-FE07695FCBB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0333A7F7-D8E7-AA49-89A0-FEDA64D0505E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="26720" windowHeight="16580" xr2:uid="{9B007B2D-73AA-3748-A695-E00E103E3607}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>N</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>ROW+1,COLUMN+1 ROW+2,COLUMN+2 ROW+3,COLUMN+3</t>
+  </si>
+  <si>
+    <t>ROW+1,COLUMN-1 ROW+2,COLUMN-2 ROW+3,COLUMN-3</t>
   </si>
 </sst>
 </file>
@@ -190,7 +193,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -270,6 +273,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -584,7 +590,7 @@
   <dimension ref="A1:U11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="U8" sqref="U8"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="6.7109375" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1050,7 +1056,9 @@
       <c r="T9" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="U9" s="23"/>
+      <c r="U9" s="27" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="10" spans="1:21" ht="46.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="str">

</xml_diff>